<commit_message>
upload data analysis code
</commit_message>
<xml_diff>
--- a/Participant Info.xlsx
+++ b/Participant Info.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tanyawen/Documents/GitHub/Difficulty-MD-network/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tanya Wen\Documents\GitHub\Difficulty-MD-network\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5167087D-75A1-7C46-86A0-6E477BD5EDA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="21620" windowHeight="15100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="21615" windowHeight="15105"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -67,9 +66,6 @@
     <t>F</t>
   </si>
   <si>
-    <t>pilot, gave participant blanket after run3</t>
-  </si>
-  <si>
     <t>s03</t>
   </si>
   <si>
@@ -191,12 +187,15 @@
   </si>
   <si>
     <t>participant has retainer on bottom row of teeth</t>
+  </si>
+  <si>
+    <t>gave participant blanket after run3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -567,19 +566,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="13.83203125" customWidth="1"/>
+    <col min="4" max="4" width="13.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -596,7 +595,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -610,10 +609,10 @@
         <v>44635</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -627,23 +626,23 @@
         <v>44649</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D4" s="1">
         <v>44655</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
@@ -655,9 +654,9 @@
         <v>44656</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
@@ -669,9 +668,9 @@
         <v>44664</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
@@ -683,23 +682,23 @@
         <v>44659</v>
       </c>
       <c r="E7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D8" s="3">
         <v>44662</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
@@ -711,12 +710,12 @@
         <v>44665</v>
       </c>
       <c r="E9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
@@ -728,9 +727,9 @@
         <v>44669</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11" t="s">
         <v>9</v>
@@ -742,9 +741,9 @@
         <v>44672</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B12" t="s">
         <v>9</v>
@@ -756,9 +755,9 @@
         <v>44687</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13" t="s">
         <v>6</v>
@@ -770,9 +769,9 @@
         <v>44690</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B14" t="s">
         <v>9</v>
@@ -784,9 +783,9 @@
         <v>44690</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B15" t="s">
         <v>6</v>
@@ -798,12 +797,12 @@
         <v>44690</v>
       </c>
       <c r="E15" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B16" t="s">
         <v>9</v>
@@ -815,9 +814,9 @@
         <v>44691</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B17" t="s">
         <v>6</v>
@@ -829,9 +828,9 @@
         <v>44693</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>9</v>
@@ -841,12 +840,12 @@
         <v>44694</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B19" t="s">
         <v>9</v>
@@ -858,9 +857,9 @@
         <v>44697</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B20" t="s">
         <v>9</v>
@@ -872,9 +871,9 @@
         <v>44697</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B21" t="s">
         <v>9</v>
@@ -886,9 +885,9 @@
         <v>44698</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>6</v>
@@ -898,12 +897,12 @@
         <v>44699</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>9</v>
@@ -913,12 +912,12 @@
         <v>44699</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B24" t="s">
         <v>9</v>
@@ -930,12 +929,12 @@
         <v>44712</v>
       </c>
       <c r="E24" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B25" t="s">
         <v>9</v>
@@ -947,9 +946,9 @@
         <v>44713</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B26" t="s">
         <v>6</v>
@@ -961,12 +960,12 @@
         <v>44714</v>
       </c>
       <c r="E26" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B27" t="s">
         <v>6</v>
@@ -978,9 +977,9 @@
         <v>44720</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B28" t="s">
         <v>9</v>
@@ -992,12 +991,12 @@
         <v>44721</v>
       </c>
       <c r="E28" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>6</v>
@@ -1009,12 +1008,12 @@
         <v>44722</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B30" t="s">
         <v>6</v>
@@ -1026,26 +1025,26 @@
         <v>44725</v>
       </c>
     </row>
-    <row r="31" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D31" s="6">
         <v>44726</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B32" t="s">
         <v>6</v>

</xml_diff>